<commit_message>
Plastic and Insulation Iterated
</commit_message>
<xml_diff>
--- a/data/calc/casing.xlsx
+++ b/data/calc/casing.xlsx
@@ -522,16 +522,16 @@
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="B2">
         <v>0.8</v>
       </c>
       <c r="C2">
-        <v>400</v>
+        <v>350</v>
       </c>
       <c r="D2">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="E2">
         <v>200</v>
@@ -552,7 +552,7 @@
         <v>1</v>
       </c>
       <c r="K2">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L2">
         <f>(((C2/1000*E2/1000)*2+(C2/1000+D2/1000)*2+(D2/1000+E2/1000)*2)+((G2/1000*I2/1000)*2+(G2/1000*H2/1000)*2+(H2/1000*I2/1000)*2))</f>

</xml_diff>

<commit_message>
Iteration upto Water Coil
</commit_message>
<xml_diff>
--- a/data/calc/casing.xlsx
+++ b/data/calc/casing.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet2" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Casing" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Coil" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>inner_sheet_thick</t>
   </si>
@@ -74,6 +75,105 @@
   </si>
   <si>
     <t>multiplying_factor</t>
+  </si>
+  <si>
+    <t>fin_height</t>
+  </si>
+  <si>
+    <t>fin_length</t>
+  </si>
+  <si>
+    <t>rd</t>
+  </si>
+  <si>
+    <t>tubes</t>
+  </si>
+  <si>
+    <t>fpi</t>
+  </si>
+  <si>
+    <t>fin_qty</t>
+  </si>
+  <si>
+    <t>tube_qty</t>
+  </si>
+  <si>
+    <t>casing_qty</t>
+  </si>
+  <si>
+    <t>header_qty</t>
+  </si>
+  <si>
+    <t>drainpan_sheet_qty</t>
+  </si>
+  <si>
+    <t>U_bend</t>
+  </si>
+  <si>
+    <t>copper_st_stub</t>
+  </si>
+  <si>
+    <t>fin_qty_f1</t>
+  </si>
+  <si>
+    <t>fin_qty_f2</t>
+  </si>
+  <si>
+    <t>casing_qty_f1</t>
+  </si>
+  <si>
+    <t>casing_qty_f2</t>
+  </si>
+  <si>
+    <t>casing_qty_f3</t>
+  </si>
+  <si>
+    <t>casing_qty_f4</t>
+  </si>
+  <si>
+    <t>casing_qty_f5</t>
+  </si>
+  <si>
+    <t>casing_qty_f6</t>
+  </si>
+  <si>
+    <t>tubes_f1</t>
+  </si>
+  <si>
+    <t>header_qty_f1</t>
+  </si>
+  <si>
+    <t>header_qty_f2</t>
+  </si>
+  <si>
+    <t>header_qty_f3</t>
+  </si>
+  <si>
+    <t>drainpan_qty_f1</t>
+  </si>
+  <si>
+    <t>drainpan_qty_f2</t>
+  </si>
+  <si>
+    <t>drainpan_qty_f3</t>
+  </si>
+  <si>
+    <t>U_bend_f1</t>
+  </si>
+  <si>
+    <t>U_bend_f2</t>
+  </si>
+  <si>
+    <t>U_bend_f3</t>
+  </si>
+  <si>
+    <t>copper_st_stub_f1</t>
+  </si>
+  <si>
+    <t>copper_st_stub_f2</t>
+  </si>
+  <si>
+    <t>meter_conv</t>
   </si>
 </sst>
 </file>
@@ -109,8 +209,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,7 +554,7 @@
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
@@ -522,19 +623,19 @@
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="B2">
         <v>0.8</v>
       </c>
       <c r="C2">
-        <v>350</v>
+        <v>1000</v>
       </c>
       <c r="D2">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="E2">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -556,37 +657,281 @@
       </c>
       <c r="L2">
         <f>(((C2/1000*E2/1000)*2+(C2/1000+D2/1000)*2+(D2/1000+E2/1000)*2)+((G2/1000*I2/1000)*2+(G2/1000*H2/1000)*2+(H2/1000*I2/1000)*2))</f>
-        <v>2.885778</v>
+        <v>6</v>
       </c>
       <c r="M2">
         <f>$A$2*L2*7.81*1.15*T2</f>
-        <v>20.734892085600002</v>
+        <v>32.33339999999999</v>
       </c>
       <c r="N2">
         <f>$B$2*L2*7.81*1.15*T2</f>
-        <v>20.734892085600002</v>
+        <v>43.111200000000004</v>
       </c>
       <c r="O2">
         <f>+((C2/1000*4)+(D2/1000*4*F2)+(E2/1000*4*F2))+((G2/1000*4)+(H2/1000*4*J2)+(I2/1000)*4*J2)</f>
-        <v>3.9960000000000004</v>
+        <v>8</v>
       </c>
       <c r="P2">
         <f>O2*0.9</f>
-        <v>3.5964000000000005</v>
+        <v>7.2</v>
       </c>
       <c r="Q2">
         <f>$L$2*40*$K$2/1000*0.6*1.1</f>
-        <v>3.6568578816</v>
+        <v>7.6032</v>
       </c>
       <c r="R2">
         <f>$L$2*40*$K$2/1000*0.4*1.1</f>
-        <v>2.4379052544000004</v>
+        <v>5.0688</v>
       </c>
       <c r="S2">
         <v>0</v>
       </c>
       <c r="T2">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="Z10" sqref="Z10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" customWidth="1"/>
+    <col min="4" max="4" width="6" customWidth="1"/>
+    <col min="5" max="5" width="3.42578125" customWidth="1"/>
+    <col min="6" max="6" width="8" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" customWidth="1"/>
+    <col min="11" max="11" width="7.85546875" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" customWidth="1"/>
+    <col min="13" max="17" width="10" customWidth="1"/>
+    <col min="18" max="20" width="13.140625" customWidth="1"/>
+    <col min="21" max="21" width="8.7109375" customWidth="1"/>
+    <col min="22" max="24" width="14" customWidth="1"/>
+    <col min="25" max="27" width="15.5703125" customWidth="1"/>
+    <col min="28" max="30" width="10.5703125" customWidth="1"/>
+    <col min="31" max="32" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W1" t="s">
+        <v>42</v>
+      </c>
+      <c r="X1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>250</v>
+      </c>
+      <c r="B2">
+        <v>460</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1">
+        <f>+A2/U2</f>
+        <v>31.496062992125985</v>
+      </c>
+      <c r="E2">
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <f>(A2/AG2)*(B2/AG2)*C2*M2*N2</f>
+        <v>34.862399999999994</v>
+      </c>
+      <c r="G2">
+        <f>(A2/AG2)*(B2/AG2)*C2*M2*N2</f>
+        <v>34.862399999999994</v>
+      </c>
+      <c r="H2">
+        <f>((A2+B2)*O2/AG2)*((C2+P2)*Q2/AG2)*R2*S2*T2</f>
+        <v>17.704332800000003</v>
+      </c>
+      <c r="I2">
+        <f>IF(AND(A2&gt;0,B2&gt;0),(A2*V2+W2)*X2/AG2,0)</f>
+        <v>4.7</v>
+      </c>
+      <c r="J2">
+        <f>IF(AND(A2&gt;0,B2&gt;0),(Y2*B2/AG2*Z2*AA2),0)</f>
+        <v>5.6232</v>
+      </c>
+      <c r="K2" s="1">
+        <f>+A2/U2*(C2*AB2-AC2)/AD2</f>
+        <v>157.48031496062993</v>
+      </c>
+      <c r="L2">
+        <f>+D2*AE2*AF2</f>
+        <v>0.9448818897637795</v>
+      </c>
+      <c r="M2">
+        <v>0.45</v>
+      </c>
+      <c r="N2">
+        <v>10.76</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>40</v>
+      </c>
+      <c r="R2">
+        <v>7.81</v>
+      </c>
+      <c r="S2">
+        <v>1.6</v>
+      </c>
+      <c r="T2">
+        <v>1.15</v>
+      </c>
+      <c r="U2">
+        <v>31.75</v>
+      </c>
+      <c r="V2">
+        <v>2</v>
+      </c>
+      <c r="W2">
+        <v>350</v>
+      </c>
+      <c r="X2">
+        <v>2</v>
+      </c>
+      <c r="Y2">
+        <v>0.6</v>
+      </c>
+      <c r="Z2">
+        <v>7.81</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+      <c r="AB2">
+        <v>2</v>
+      </c>
+      <c r="AC2">
+        <v>2</v>
+      </c>
+      <c r="AD2">
+        <v>2</v>
+      </c>
+      <c r="AE2">
+        <v>2</v>
+      </c>
+      <c r="AF2">
+        <v>0.015</v>
+      </c>
+      <c r="AG2">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>